<commit_message>
update stock transfering all related featured
</commit_message>
<xml_diff>
--- a/public/backend/file/order_import.xlsx
+++ b/public/backend/file/order_import.xlsx
@@ -12,36 +12,40 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Contacts" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>name</t>
+  </si>
   <si>
     <t>quantity</t>
   </si>
   <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>diameter</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>B05</t>
-  </si>
-  <si>
-    <t>Standard</t>
+    <t>E23-11-Premium</t>
+  </si>
+  <si>
+    <t>E25-11-Premium</t>
+  </si>
+  <si>
+    <t>E27-11.2-Premium</t>
+  </si>
+  <si>
+    <t>E28-11.2-Premium</t>
+  </si>
+  <si>
+    <t>E29-11.2-Premium</t>
+  </si>
+  <si>
+    <t>E08-10.4-Premium</t>
+  </si>
+  <si>
+    <t>serials</t>
   </si>
 </sst>
 </file>
@@ -51,17 +55,14 @@
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Arial"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -73,8 +74,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FF305496"/>
       </patternFill>
     </fill>
   </fills>
@@ -98,7 +98,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -373,50 +373,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.109375" customWidth="1"/>
-    <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
-        <v>11.4</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="D2">
-        <v>5</v>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[update] order detail: import file
</commit_message>
<xml_diff>
--- a/public/backend/file/order_import.xlsx
+++ b/public/backend/file/order_import.xlsx
@@ -5,24 +5,143 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luanp\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hungnt\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
-    <sheet name="Contacts" sheetId="1" r:id="rId1"/>
+    <sheet name="order details" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Hung Nguyen</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tên sản phẩm: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tên sản phẩm phải tồn tại trên hệ thống</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Số lô</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Kho: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tên kho phải tồn tại trên hệ thống; 
+Lưu ý: Nếu kho không tồn tại trên hệ thống, thì hệ thống sẽ lấy mặc định theo thông tin kho hàng mặc định của đơn hàng.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Số lượng: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Số lượng phải thuộc kiểu số dương</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Đơn giá bán/mua</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Số tiền giảm giá</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>quantity</t>
   </si>
@@ -46,23 +165,78 @@
   </si>
   <si>
     <t>serials</t>
+  </si>
+  <si>
+    <t>product name</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>discount</t>
+  </si>
+  <si>
+    <t>Lô A</t>
+  </si>
+  <si>
+    <t>Lô 2</t>
+  </si>
+  <si>
+    <t>Lô C</t>
+  </si>
+  <si>
+    <t>Lô 1A</t>
+  </si>
+  <si>
+    <t>Lô 2A</t>
+  </si>
+  <si>
+    <t>Lô 1B</t>
+  </si>
+  <si>
+    <t>warehouse</t>
+  </si>
+  <si>
+    <t>SG</t>
+  </si>
+  <si>
+    <t>Kho Hi-Tech</t>
+  </si>
+  <si>
+    <t>HN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="1"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -74,7 +248,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF305496"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -90,9 +265,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,79 +556,152 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.8984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.8984375" customWidth="1"/>
+    <col min="2" max="3" width="14.19921875" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.3984375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1">
+        <v>800000</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
         <v>1</v>
       </c>
+      <c r="E3" s="1">
+        <v>2000000</v>
+      </c>
+      <c r="F3" s="1">
+        <v>200000</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
         <v>1</v>
       </c>
+      <c r="E4" s="1">
+        <v>2900000</v>
+      </c>
+      <c r="F4" s="1">
+        <v>100000</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6">
         <v>1</v>
       </c>
+      <c r="E6" s="1">
+        <v>1500000</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
+      <c r="E7" s="1">
+        <v>1500000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>